<commit_message>
Basic excel cleaning done
</commit_message>
<xml_diff>
--- a/Excel/HRDataset_v14 - Working.xlsx
+++ b/Excel/HRDataset_v14 - Working.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\Desktop\Data analyst portfolio projects\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{D85714BC-FA8B-46FA-AEE5-C9341EEAE79D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{314C0EB3-C8D9-4F33-A002-CED7FA285463}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{FAE3CAE8-3C73-43C1-9511-3278F5C7C99C}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8780" uniqueCount="488">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8987" uniqueCount="489">
   <si>
     <t>Employee_Name</t>
   </si>
@@ -1496,6 +1496,9 @@
   <si>
     <t>Zima, Colleen</t>
   </si>
+  <si>
+    <t>NULL</t>
+  </si>
 </sst>
 </file>
 
@@ -1986,10 +1989,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -36057,8 +36061,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C1C7566-FF8C-4B87-AFAC-D0B14E4AA402}">
   <dimension ref="A1:AJ312"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
-      <selection activeCell="AB21" sqref="AB21:AB253"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="U1" sqref="U1:U1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -36078,14 +36082,14 @@
     <col min="13" max="13" width="25.5546875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="5.77734375" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="6" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="27.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="4.33203125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="12.109375" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="15.88671875" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="15" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="27.5546875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="18.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="25.44140625" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="19.109375" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="18" bestFit="1" customWidth="1"/>
@@ -36096,7 +36100,7 @@
     <col min="31" max="31" width="18.88671875" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="16.21875" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="21.44140625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="29" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="29" style="1" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="15.5546875" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="10" bestFit="1" customWidth="1"/>
   </cols>
@@ -36147,7 +36151,7 @@
       <c r="O1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="P1" s="3" t="s">
         <v>15</v>
       </c>
       <c r="Q1" s="2" t="s">
@@ -36165,10 +36169,10 @@
       <c r="U1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="V1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="W1" s="3" t="s">
         <v>22</v>
       </c>
       <c r="X1" s="2" t="s">
@@ -36201,7 +36205,7 @@
       <c r="AG1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="2" t="s">
+      <c r="AH1" s="3" t="s">
         <v>33</v>
       </c>
       <c r="AI1" s="2" t="s">
@@ -36278,6 +36282,9 @@
       <c r="V2" s="1">
         <v>40729</v>
       </c>
+      <c r="W2" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X2" t="s">
         <v>44</v>
       </c>
@@ -36605,6 +36612,9 @@
       <c r="V5" s="1">
         <v>39454</v>
       </c>
+      <c r="W5" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X5" t="s">
         <v>44</v>
       </c>
@@ -36822,6 +36832,9 @@
       <c r="V7" s="1">
         <v>40917</v>
       </c>
+      <c r="W7" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X7" t="s">
         <v>44</v>
       </c>
@@ -36929,6 +36942,9 @@
       <c r="V8" s="1">
         <v>41953</v>
       </c>
+      <c r="W8" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X8" t="s">
         <v>44</v>
       </c>
@@ -37036,6 +37052,9 @@
       <c r="V9" s="1">
         <v>41547</v>
       </c>
+      <c r="W9" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X9" t="s">
         <v>44</v>
       </c>
@@ -37143,6 +37162,9 @@
       <c r="V10" s="1">
         <v>40000</v>
       </c>
+      <c r="W10" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X10" t="s">
         <v>44</v>
       </c>
@@ -37250,6 +37272,9 @@
       <c r="V11" s="1">
         <v>42009</v>
       </c>
+      <c r="W11" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X11" t="s">
         <v>44</v>
       </c>
@@ -37577,6 +37602,9 @@
       <c r="V14" s="1">
         <v>41953</v>
       </c>
+      <c r="W14" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X14" t="s">
         <v>44</v>
       </c>
@@ -37684,6 +37712,9 @@
       <c r="V15" s="1">
         <v>40959</v>
       </c>
+      <c r="W15" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X15" t="s">
         <v>44</v>
       </c>
@@ -38011,6 +38042,9 @@
       <c r="V18" s="1">
         <v>42572</v>
       </c>
+      <c r="W18" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X18" t="s">
         <v>44</v>
       </c>
@@ -38118,6 +38152,9 @@
       <c r="V19" s="1">
         <v>40637</v>
       </c>
+      <c r="W19" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X19" t="s">
         <v>44</v>
       </c>
@@ -38335,6 +38372,9 @@
       <c r="V21" s="1">
         <v>41463</v>
       </c>
+      <c r="W21" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X21" t="s">
         <v>44</v>
       </c>
@@ -38442,6 +38482,9 @@
       <c r="V22" s="1">
         <v>41001</v>
       </c>
+      <c r="W22" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X22" t="s">
         <v>44</v>
       </c>
@@ -38549,6 +38592,9 @@
       <c r="V23" s="1">
         <v>41505</v>
       </c>
+      <c r="W23" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X23" t="s">
         <v>44</v>
       </c>
@@ -38656,6 +38702,9 @@
       <c r="V24" s="1">
         <v>41827</v>
       </c>
+      <c r="W24" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X24" t="s">
         <v>44</v>
       </c>
@@ -38763,6 +38812,9 @@
       <c r="V25" s="1">
         <v>40637</v>
       </c>
+      <c r="W25" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X25" t="s">
         <v>44</v>
       </c>
@@ -39090,6 +39142,9 @@
       <c r="V28" s="1">
         <v>42051</v>
       </c>
+      <c r="W28" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X28" t="s">
         <v>44</v>
       </c>
@@ -39417,6 +39472,9 @@
       <c r="V31" s="1">
         <v>39748</v>
       </c>
+      <c r="W31" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X31" t="s">
         <v>44</v>
       </c>
@@ -39524,6 +39582,9 @@
       <c r="V32" s="1">
         <v>41911</v>
       </c>
+      <c r="W32" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X32" t="s">
         <v>44</v>
       </c>
@@ -39631,6 +39692,9 @@
       <c r="V33" s="1">
         <v>41589</v>
       </c>
+      <c r="W33" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X33" t="s">
         <v>44</v>
       </c>
@@ -39848,6 +39912,9 @@
       <c r="V35" s="1">
         <v>40973</v>
       </c>
+      <c r="W35" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X35" t="s">
         <v>44</v>
       </c>
@@ -39955,6 +40022,9 @@
       <c r="V36" s="1">
         <v>40637</v>
       </c>
+      <c r="W36" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X36" t="s">
         <v>44</v>
       </c>
@@ -40062,6 +40132,9 @@
       <c r="V37" s="1">
         <v>40770</v>
       </c>
+      <c r="W37" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X37" t="s">
         <v>44</v>
       </c>
@@ -40169,6 +40242,9 @@
       <c r="V38" s="1">
         <v>42397</v>
       </c>
+      <c r="W38" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X38" t="s">
         <v>44</v>
       </c>
@@ -40276,6 +40352,9 @@
       <c r="V39" s="1">
         <v>41589</v>
       </c>
+      <c r="W39" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X39" t="s">
         <v>44</v>
       </c>
@@ -40383,6 +40462,9 @@
       <c r="V40" s="1">
         <v>41729</v>
       </c>
+      <c r="W40" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X40" t="s">
         <v>44</v>
       </c>
@@ -40490,6 +40572,9 @@
       <c r="V41" s="1">
         <v>42551</v>
       </c>
+      <c r="W41" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X41" t="s">
         <v>44</v>
       </c>
@@ -40597,6 +40682,9 @@
       <c r="V42" s="1">
         <v>41869</v>
       </c>
+      <c r="W42" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X42" t="s">
         <v>44</v>
       </c>
@@ -40704,6 +40792,9 @@
       <c r="V43" s="1">
         <v>41911</v>
       </c>
+      <c r="W43" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X43" t="s">
         <v>44</v>
       </c>
@@ -40811,6 +40902,9 @@
       <c r="V44" s="1">
         <v>42619</v>
       </c>
+      <c r="W44" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X44" t="s">
         <v>44</v>
       </c>
@@ -40918,6 +41012,9 @@
       <c r="V45" s="1">
         <v>41771</v>
       </c>
+      <c r="W45" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X45" t="s">
         <v>44</v>
       </c>
@@ -41025,6 +41122,9 @@
       <c r="V46" s="1">
         <v>41463</v>
       </c>
+      <c r="W46" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X46" t="s">
         <v>44</v>
       </c>
@@ -41132,6 +41232,9 @@
       <c r="V47" s="1">
         <v>41043</v>
       </c>
+      <c r="W47" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X47" t="s">
         <v>44</v>
       </c>
@@ -41349,6 +41452,9 @@
       <c r="V49" s="1">
         <v>40819</v>
       </c>
+      <c r="W49" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X49" t="s">
         <v>44</v>
       </c>
@@ -41456,6 +41562,9 @@
       <c r="V50" s="1">
         <v>41157</v>
       </c>
+      <c r="W50" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X50" t="s">
         <v>44</v>
       </c>
@@ -41783,6 +41892,9 @@
       <c r="V53" s="1">
         <v>42557</v>
       </c>
+      <c r="W53" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X53" t="s">
         <v>44</v>
       </c>
@@ -41890,6 +42002,9 @@
       <c r="V54" s="1">
         <v>41463</v>
       </c>
+      <c r="W54" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X54" t="s">
         <v>44</v>
       </c>
@@ -42107,6 +42222,9 @@
       <c r="V56" s="1">
         <v>40379</v>
       </c>
+      <c r="W56" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X56" t="s">
         <v>44</v>
       </c>
@@ -42214,6 +42332,9 @@
       <c r="V57" s="1">
         <v>39818</v>
       </c>
+      <c r="W57" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X57" t="s">
         <v>44</v>
       </c>
@@ -42321,6 +42442,9 @@
       <c r="V58" s="1">
         <v>42009</v>
       </c>
+      <c r="W58" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X58" t="s">
         <v>44</v>
       </c>
@@ -42428,6 +42552,9 @@
       <c r="V59" s="1">
         <v>42093</v>
       </c>
+      <c r="W59" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X59" t="s">
         <v>44</v>
       </c>
@@ -42535,6 +42662,9 @@
       <c r="V60" s="1">
         <v>42557</v>
       </c>
+      <c r="W60" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X60" t="s">
         <v>44</v>
       </c>
@@ -42642,6 +42772,9 @@
       <c r="V61" s="1">
         <v>41953</v>
       </c>
+      <c r="W61" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X61" t="s">
         <v>44</v>
       </c>
@@ -42749,6 +42882,9 @@
       <c r="V62" s="1">
         <v>41764</v>
       </c>
+      <c r="W62" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X62" t="s">
         <v>44</v>
       </c>
@@ -42856,6 +42992,9 @@
       <c r="V63" s="1">
         <v>41953</v>
       </c>
+      <c r="W63" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X63" t="s">
         <v>44</v>
       </c>
@@ -42963,6 +43102,9 @@
       <c r="V64" s="1">
         <v>41092</v>
       </c>
+      <c r="W64" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X64" t="s">
         <v>44</v>
       </c>
@@ -43070,6 +43212,9 @@
       <c r="V65" s="1">
         <v>40854</v>
       </c>
+      <c r="W65" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X65" t="s">
         <v>44</v>
       </c>
@@ -43177,6 +43322,9 @@
       <c r="V66" s="1">
         <v>43290</v>
       </c>
+      <c r="W66" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X66" t="s">
         <v>44</v>
       </c>
@@ -43394,6 +43542,9 @@
       <c r="V68" s="1">
         <v>40917</v>
       </c>
+      <c r="W68" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X68" t="s">
         <v>44</v>
       </c>
@@ -43501,6 +43652,9 @@
       <c r="V69" s="1">
         <v>41911</v>
       </c>
+      <c r="W69" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X69" t="s">
         <v>44</v>
       </c>
@@ -43718,6 +43872,9 @@
       <c r="V71" s="1">
         <v>41827</v>
       </c>
+      <c r="W71" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X71" t="s">
         <v>44</v>
       </c>
@@ -43825,6 +43982,9 @@
       <c r="V72" s="1">
         <v>42781</v>
       </c>
+      <c r="W72" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X72" t="s">
         <v>44</v>
       </c>
@@ -43932,6 +44092,9 @@
       <c r="V73" s="1">
         <v>41771</v>
       </c>
+      <c r="W73" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X73" t="s">
         <v>44</v>
       </c>
@@ -44039,6 +44202,9 @@
       <c r="V74" s="1">
         <v>40959</v>
       </c>
+      <c r="W74" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X74" t="s">
         <v>44</v>
       </c>
@@ -44146,6 +44312,9 @@
       <c r="V75" s="1">
         <v>41281</v>
       </c>
+      <c r="W75" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X75" t="s">
         <v>44</v>
       </c>
@@ -44253,6 +44422,9 @@
       <c r="V76" s="1">
         <v>41001</v>
       </c>
+      <c r="W76" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X76" t="s">
         <v>44</v>
       </c>
@@ -44360,6 +44532,9 @@
       <c r="V77" s="1">
         <v>42009</v>
       </c>
+      <c r="W77" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X77" t="s">
         <v>44</v>
       </c>
@@ -44467,6 +44642,9 @@
       <c r="V78" s="1">
         <v>41644</v>
       </c>
+      <c r="W78" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X78" t="s">
         <v>44</v>
       </c>
@@ -44574,6 +44752,9 @@
       <c r="V79" s="1">
         <v>40553</v>
       </c>
+      <c r="W79" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X79" t="s">
         <v>44</v>
       </c>
@@ -44681,6 +44862,9 @@
       <c r="V80" s="1">
         <v>41900</v>
       </c>
+      <c r="W80" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X80" t="s">
         <v>44</v>
       </c>
@@ -44788,6 +44972,9 @@
       <c r="V81" s="1">
         <v>40294</v>
       </c>
+      <c r="W81" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X81" t="s">
         <v>44</v>
       </c>
@@ -45005,6 +45192,9 @@
       <c r="V83" s="1">
         <v>41953</v>
       </c>
+      <c r="W83" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X83" t="s">
         <v>44</v>
       </c>
@@ -45112,6 +45302,9 @@
       <c r="V84" s="1">
         <v>41729</v>
       </c>
+      <c r="W84" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X84" t="s">
         <v>44</v>
       </c>
@@ -45219,6 +45412,9 @@
       <c r="V85" s="1">
         <v>41827</v>
       </c>
+      <c r="W85" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X85" t="s">
         <v>44</v>
       </c>
@@ -45656,6 +45852,9 @@
       <c r="V89" s="1">
         <v>41827</v>
       </c>
+      <c r="W89" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X89" t="s">
         <v>44</v>
       </c>
@@ -45763,6 +45962,9 @@
       <c r="V90" s="1">
         <v>41687</v>
       </c>
+      <c r="W90" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X90" t="s">
         <v>44</v>
       </c>
@@ -45980,6 +46182,9 @@
       <c r="V92" s="1">
         <v>42135</v>
       </c>
+      <c r="W92" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X92" t="s">
         <v>44</v>
       </c>
@@ -46087,6 +46292,9 @@
       <c r="V93" s="1">
         <v>42093</v>
       </c>
+      <c r="W93" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X93" t="s">
         <v>44</v>
       </c>
@@ -46194,6 +46402,9 @@
       <c r="V94" s="1">
         <v>40917</v>
       </c>
+      <c r="W94" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X94" t="s">
         <v>44</v>
       </c>
@@ -46631,6 +46842,9 @@
       <c r="V98" s="1">
         <v>40648</v>
       </c>
+      <c r="W98" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X98" t="s">
         <v>44</v>
       </c>
@@ -46738,6 +46952,9 @@
       <c r="V99" s="1">
         <v>39818</v>
       </c>
+      <c r="W99" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X99" t="s">
         <v>44</v>
       </c>
@@ -46845,6 +47062,9 @@
       <c r="V100" s="1">
         <v>40792</v>
       </c>
+      <c r="W100" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X100" t="s">
         <v>44</v>
       </c>
@@ -46952,6 +47172,9 @@
       <c r="V101" s="1">
         <v>40299</v>
       </c>
+      <c r="W101" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X101" t="s">
         <v>44</v>
       </c>
@@ -47059,6 +47282,9 @@
       <c r="V102" s="1">
         <v>42093</v>
       </c>
+      <c r="W102" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X102" t="s">
         <v>44</v>
       </c>
@@ -47166,6 +47392,9 @@
       <c r="V103" s="1">
         <v>40679</v>
       </c>
+      <c r="W103" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X103" t="s">
         <v>44</v>
       </c>
@@ -47273,6 +47502,9 @@
       <c r="V104" s="1">
         <v>42093</v>
       </c>
+      <c r="W104" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X104" t="s">
         <v>44</v>
       </c>
@@ -47710,6 +47942,9 @@
       <c r="V108" s="1">
         <v>41911</v>
       </c>
+      <c r="W108" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X108" t="s">
         <v>44</v>
       </c>
@@ -47817,6 +48052,9 @@
       <c r="V109" s="1">
         <v>42051</v>
       </c>
+      <c r="W109" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X109" t="s">
         <v>44</v>
       </c>
@@ -48034,6 +48272,9 @@
       <c r="V111" s="1">
         <v>42093</v>
       </c>
+      <c r="W111" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X111" t="s">
         <v>44</v>
       </c>
@@ -48141,6 +48382,9 @@
       <c r="V112" s="1">
         <v>41589</v>
       </c>
+      <c r="W112" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X112" t="s">
         <v>44</v>
       </c>
@@ -48248,6 +48492,9 @@
       <c r="V113" s="1">
         <v>40735</v>
       </c>
+      <c r="W113" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X113" t="s">
         <v>44</v>
       </c>
@@ -48465,6 +48712,9 @@
       <c r="V115" s="1">
         <v>42009</v>
       </c>
+      <c r="W115" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X115" t="s">
         <v>44</v>
       </c>
@@ -48572,6 +48822,9 @@
       <c r="V116" s="1">
         <v>41771</v>
       </c>
+      <c r="W116" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X116" t="s">
         <v>44</v>
       </c>
@@ -48679,6 +48932,9 @@
       <c r="V117" s="1">
         <v>41092</v>
       </c>
+      <c r="W117" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X117" t="s">
         <v>44</v>
       </c>
@@ -48786,6 +49042,9 @@
       <c r="V118" s="1">
         <v>41547</v>
       </c>
+      <c r="W118" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X118" t="s">
         <v>44</v>
       </c>
@@ -48893,6 +49152,9 @@
       <c r="V119" s="1">
         <v>41505</v>
       </c>
+      <c r="W119" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X119" t="s">
         <v>44</v>
       </c>
@@ -49000,6 +49262,9 @@
       <c r="V120" s="1">
         <v>42157</v>
       </c>
+      <c r="W120" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X120" t="s">
         <v>44</v>
       </c>
@@ -49217,6 +49482,9 @@
       <c r="V122" s="1">
         <v>42845</v>
       </c>
+      <c r="W122" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X122" t="s">
         <v>44</v>
       </c>
@@ -49434,6 +49702,9 @@
       <c r="V124" s="1">
         <v>40875</v>
       </c>
+      <c r="W124" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X124" t="s">
         <v>44</v>
       </c>
@@ -49541,6 +49812,9 @@
       <c r="V125" s="1">
         <v>41589</v>
       </c>
+      <c r="W125" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X125" t="s">
         <v>44</v>
       </c>
@@ -49758,6 +50032,9 @@
       <c r="V127" s="1">
         <v>41771</v>
       </c>
+      <c r="W127" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X127" t="s">
         <v>44</v>
       </c>
@@ -49865,6 +50142,9 @@
       <c r="V128" s="1">
         <v>41134</v>
       </c>
+      <c r="W128" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X128" t="s">
         <v>44</v>
       </c>
@@ -50082,6 +50362,9 @@
       <c r="V130" s="1">
         <v>41869</v>
       </c>
+      <c r="W130" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X130" t="s">
         <v>44</v>
       </c>
@@ -50299,6 +50582,9 @@
       <c r="V132" s="1">
         <v>42093</v>
       </c>
+      <c r="W132" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X132" t="s">
         <v>44</v>
       </c>
@@ -50406,6 +50692,9 @@
       <c r="V133" s="1">
         <v>41764</v>
       </c>
+      <c r="W133" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X133" t="s">
         <v>44</v>
       </c>
@@ -50623,6 +50912,9 @@
       <c r="V135" s="1">
         <v>40959</v>
       </c>
+      <c r="W135" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X135" t="s">
         <v>44</v>
       </c>
@@ -50730,6 +51022,9 @@
       <c r="V136" s="1">
         <v>42527</v>
       </c>
+      <c r="W136" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X136" t="s">
         <v>44</v>
       </c>
@@ -50837,6 +51132,9 @@
       <c r="V137" s="1">
         <v>42160</v>
       </c>
+      <c r="W137" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X137" t="s">
         <v>44</v>
       </c>
@@ -51164,6 +51462,9 @@
       <c r="V140" s="1">
         <v>41505</v>
       </c>
+      <c r="W140" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X140" t="s">
         <v>44</v>
       </c>
@@ -51271,6 +51572,9 @@
       <c r="V141" s="1">
         <v>41218</v>
       </c>
+      <c r="W141" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X141" t="s">
         <v>44</v>
       </c>
@@ -51378,6 +51682,9 @@
       <c r="V142" s="1">
         <v>41547</v>
       </c>
+      <c r="W142" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X142" t="s">
         <v>44</v>
       </c>
@@ -51485,6 +51792,9 @@
       <c r="V143" s="1">
         <v>40729</v>
       </c>
+      <c r="W143" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X143" t="s">
         <v>44</v>
       </c>
@@ -51592,6 +51902,9 @@
       <c r="V144" s="1">
         <v>41645</v>
       </c>
+      <c r="W144" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X144" t="s">
         <v>44</v>
       </c>
@@ -51809,6 +52122,9 @@
       <c r="V146" s="1">
         <v>42009</v>
       </c>
+      <c r="W146" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X146" t="s">
         <v>44</v>
       </c>
@@ -51916,6 +52232,9 @@
       <c r="V147" s="1">
         <v>41827</v>
       </c>
+      <c r="W147" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X147" t="s">
         <v>44</v>
       </c>
@@ -52243,6 +52562,9 @@
       <c r="V150" s="1">
         <v>41547</v>
       </c>
+      <c r="W150" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X150" t="s">
         <v>44</v>
       </c>
@@ -52350,6 +52672,9 @@
       <c r="V151" s="1">
         <v>41505</v>
       </c>
+      <c r="W151" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X151" t="s">
         <v>44</v>
       </c>
@@ -52457,6 +52782,9 @@
       <c r="V152" s="1">
         <v>41092</v>
       </c>
+      <c r="W152" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X152" t="s">
         <v>44</v>
       </c>
@@ -52784,6 +53112,9 @@
       <c r="V155" s="1">
         <v>41687</v>
       </c>
+      <c r="W155" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X155" t="s">
         <v>44</v>
       </c>
@@ -52891,6 +53222,9 @@
       <c r="V156" s="1">
         <v>40553</v>
       </c>
+      <c r="W156" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X156" t="s">
         <v>44</v>
       </c>
@@ -52998,6 +53332,9 @@
       <c r="V157" s="1">
         <v>40609</v>
       </c>
+      <c r="W157" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X157" t="s">
         <v>44</v>
       </c>
@@ -53105,6 +53442,9 @@
       <c r="V158" s="1">
         <v>41953</v>
       </c>
+      <c r="W158" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X158" t="s">
         <v>44</v>
       </c>
@@ -53432,6 +53772,9 @@
       <c r="V161" s="1">
         <v>41099</v>
       </c>
+      <c r="W161" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X161" t="s">
         <v>44</v>
       </c>
@@ -53539,6 +53882,9 @@
       <c r="V162" s="1">
         <v>41645</v>
       </c>
+      <c r="W162" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X162" t="s">
         <v>44</v>
       </c>
@@ -53756,6 +54102,9 @@
       <c r="V164" s="1">
         <v>42645</v>
       </c>
+      <c r="W164" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X164" t="s">
         <v>44</v>
       </c>
@@ -53973,6 +54322,9 @@
       <c r="V166" s="1">
         <v>42374</v>
       </c>
+      <c r="W166" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X166" t="s">
         <v>44</v>
       </c>
@@ -54080,6 +54432,9 @@
       <c r="V167" s="1">
         <v>41043</v>
       </c>
+      <c r="W167" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X167" t="s">
         <v>44</v>
       </c>
@@ -54187,6 +54542,9 @@
       <c r="V168" s="1">
         <v>41029</v>
       </c>
+      <c r="W168" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X168" t="s">
         <v>44</v>
       </c>
@@ -54294,6 +54652,9 @@
       <c r="V169" s="1">
         <v>41547</v>
       </c>
+      <c r="W169" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X169" t="s">
         <v>44</v>
       </c>
@@ -54511,6 +54872,9 @@
       <c r="V171" s="1">
         <v>41463</v>
       </c>
+      <c r="W171" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X171" t="s">
         <v>44</v>
       </c>
@@ -54618,6 +54982,9 @@
       <c r="V172" s="1">
         <v>40564</v>
       </c>
+      <c r="W172" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X172" t="s">
         <v>44</v>
       </c>
@@ -54835,6 +55202,9 @@
       <c r="V174" s="1">
         <v>41505</v>
       </c>
+      <c r="W174" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X174" t="s">
         <v>44</v>
       </c>
@@ -54942,6 +55312,9 @@
       <c r="V175" s="1">
         <v>42051</v>
       </c>
+      <c r="W175" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X175" t="s">
         <v>44</v>
       </c>
@@ -55269,6 +55642,9 @@
       <c r="V178" s="1">
         <v>41645</v>
       </c>
+      <c r="W178" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X178" t="s">
         <v>44</v>
       </c>
@@ -55376,6 +55752,9 @@
       <c r="V179" s="1">
         <v>42501</v>
       </c>
+      <c r="W179" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X179" t="s">
         <v>44</v>
       </c>
@@ -55593,6 +55972,9 @@
       <c r="V181" s="1">
         <v>41589</v>
       </c>
+      <c r="W181" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X181" t="s">
         <v>44</v>
       </c>
@@ -55700,6 +56082,9 @@
       <c r="V182" s="1">
         <v>41589</v>
       </c>
+      <c r="W182" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X182" t="s">
         <v>44</v>
       </c>
@@ -55807,6 +56192,9 @@
       <c r="V183" s="1">
         <v>40694</v>
       </c>
+      <c r="W183" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X183" t="s">
         <v>44</v>
       </c>
@@ -55914,6 +56302,9 @@
       <c r="V184" s="1">
         <v>42093</v>
       </c>
+      <c r="W184" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X184" t="s">
         <v>44</v>
       </c>
@@ -56021,6 +56412,9 @@
       <c r="V185" s="1">
         <v>41281</v>
       </c>
+      <c r="W185" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X185" t="s">
         <v>44</v>
       </c>
@@ -56128,6 +56522,9 @@
       <c r="V186" s="1">
         <v>42557</v>
       </c>
+      <c r="W186" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X186" t="s">
         <v>44</v>
       </c>
@@ -56345,6 +56742,9 @@
       <c r="V188" s="1">
         <v>42093</v>
       </c>
+      <c r="W188" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X188" t="s">
         <v>44</v>
       </c>
@@ -56452,6 +56852,9 @@
       <c r="V189" s="1">
         <v>41137</v>
       </c>
+      <c r="W189" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X189" t="s">
         <v>44</v>
       </c>
@@ -56669,6 +57072,9 @@
       <c r="V191" s="1">
         <v>40854</v>
       </c>
+      <c r="W191" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X191" t="s">
         <v>44</v>
       </c>
@@ -56776,6 +57182,9 @@
       <c r="V192" s="1">
         <v>40954</v>
       </c>
+      <c r="W192" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X192" t="s">
         <v>44</v>
       </c>
@@ -56883,6 +57292,9 @@
       <c r="V193" s="1">
         <v>41407</v>
       </c>
+      <c r="W193" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X193" t="s">
         <v>44</v>
       </c>
@@ -56990,6 +57402,9 @@
       <c r="V194" s="1">
         <v>40917</v>
       </c>
+      <c r="W194" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X194" t="s">
         <v>44</v>
       </c>
@@ -57097,6 +57512,9 @@
       <c r="V195" s="1">
         <v>42051</v>
       </c>
+      <c r="W195" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X195" t="s">
         <v>44</v>
       </c>
@@ -57204,6 +57622,9 @@
       <c r="V196" s="1">
         <v>41365</v>
       </c>
+      <c r="W196" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X196" t="s">
         <v>44</v>
       </c>
@@ -57311,6 +57732,9 @@
       <c r="V197" s="1">
         <v>41407</v>
       </c>
+      <c r="W197" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X197" t="s">
         <v>44</v>
       </c>
@@ -57418,6 +57842,9 @@
       <c r="V198" s="1">
         <v>41463</v>
       </c>
+      <c r="W198" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X198" t="s">
         <v>44</v>
       </c>
@@ -57525,6 +57952,9 @@
       <c r="V199" s="1">
         <v>42776</v>
       </c>
+      <c r="W199" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X199" t="s">
         <v>44</v>
       </c>
@@ -57852,6 +58282,9 @@
       <c r="V202" s="1">
         <v>41771</v>
       </c>
+      <c r="W202" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X202" t="s">
         <v>44</v>
       </c>
@@ -57959,6 +58392,9 @@
       <c r="V203" s="1">
         <v>41365</v>
       </c>
+      <c r="W203" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X203" t="s">
         <v>44</v>
       </c>
@@ -58066,6 +58502,9 @@
       <c r="V204" s="1">
         <v>41463</v>
       </c>
+      <c r="W204" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X204" t="s">
         <v>44</v>
       </c>
@@ -58173,6 +58612,9 @@
       <c r="V205" s="1">
         <v>41463</v>
       </c>
+      <c r="W205" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X205" t="s">
         <v>44</v>
       </c>
@@ -58280,6 +58722,9 @@
       <c r="V206" s="1">
         <v>41953</v>
       </c>
+      <c r="W206" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X206" t="s">
         <v>44</v>
       </c>
@@ -58607,6 +59052,9 @@
       <c r="V209" s="1">
         <v>41547</v>
       </c>
+      <c r="W209" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X209" t="s">
         <v>44</v>
       </c>
@@ -58714,6 +59162,9 @@
       <c r="V210" s="1">
         <v>41547</v>
       </c>
+      <c r="W210" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X210" t="s">
         <v>44</v>
       </c>
@@ -58821,6 +59272,9 @@
       <c r="V211" s="1">
         <v>41687</v>
       </c>
+      <c r="W211" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X211" t="s">
         <v>44</v>
       </c>
@@ -58928,6 +59382,9 @@
       <c r="V212" s="1">
         <v>42009</v>
       </c>
+      <c r="W212" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X212" t="s">
         <v>44</v>
       </c>
@@ -59915,6 +60372,9 @@
       <c r="V221" s="1">
         <v>41001</v>
       </c>
+      <c r="W221" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X221" t="s">
         <v>44</v>
       </c>
@@ -60022,6 +60482,9 @@
       <c r="V222" s="1">
         <v>41953</v>
       </c>
+      <c r="W222" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X222" t="s">
         <v>44</v>
       </c>
@@ -60239,6 +60702,9 @@
       <c r="V224" s="1">
         <v>39391</v>
       </c>
+      <c r="W224" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X224" t="s">
         <v>44</v>
       </c>
@@ -60346,6 +60812,9 @@
       <c r="V225" s="1">
         <v>40917</v>
       </c>
+      <c r="W225" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X225" t="s">
         <v>44</v>
       </c>
@@ -60563,6 +61032,9 @@
       <c r="V227" s="1">
         <v>41645</v>
       </c>
+      <c r="W227" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X227" t="s">
         <v>44</v>
       </c>
@@ -60890,6 +61362,9 @@
       <c r="V230" s="1">
         <v>42645</v>
       </c>
+      <c r="W230" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X230" t="s">
         <v>44</v>
       </c>
@@ -61107,6 +61582,9 @@
       <c r="V232" s="1">
         <v>41771</v>
       </c>
+      <c r="W232" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X232" t="s">
         <v>44</v>
       </c>
@@ -61324,6 +61802,9 @@
       <c r="V234" s="1">
         <v>40875</v>
       </c>
+      <c r="W234" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X234" t="s">
         <v>44</v>
       </c>
@@ -61871,6 +62352,9 @@
       <c r="V239" s="1">
         <v>41463</v>
       </c>
+      <c r="W239" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X239" t="s">
         <v>44</v>
       </c>
@@ -61978,6 +62462,9 @@
       <c r="V240" s="1">
         <v>42051</v>
       </c>
+      <c r="W240" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X240" t="s">
         <v>44</v>
       </c>
@@ -62195,6 +62682,9 @@
       <c r="V242" s="1">
         <v>42742</v>
       </c>
+      <c r="W242" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X242" t="s">
         <v>44</v>
       </c>
@@ -62302,6 +62792,9 @@
       <c r="V243" s="1">
         <v>41645</v>
       </c>
+      <c r="W243" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X243" t="s">
         <v>44</v>
       </c>
@@ -62519,6 +63012,9 @@
       <c r="V245" s="1">
         <v>41294</v>
       </c>
+      <c r="W245" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X245" t="s">
         <v>44</v>
       </c>
@@ -62736,6 +63232,9 @@
       <c r="V247" s="1">
         <v>41218</v>
       </c>
+      <c r="W247" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X247" t="s">
         <v>44</v>
       </c>
@@ -62843,6 +63342,9 @@
       <c r="V248" s="1">
         <v>42555</v>
       </c>
+      <c r="W248" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X248" t="s">
         <v>44</v>
       </c>
@@ -63060,6 +63562,9 @@
       <c r="V250" s="1">
         <v>40420</v>
       </c>
+      <c r="W250" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X250" t="s">
         <v>44</v>
       </c>
@@ -63277,6 +63782,9 @@
       <c r="V252" s="1">
         <v>41911</v>
       </c>
+      <c r="W252" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X252" t="s">
         <v>44</v>
       </c>
@@ -63384,6 +63892,9 @@
       <c r="V253" s="1">
         <v>41547</v>
       </c>
+      <c r="W253" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X253" t="s">
         <v>44</v>
       </c>
@@ -63491,6 +64002,9 @@
       <c r="V254" s="1">
         <v>41912</v>
       </c>
+      <c r="W254" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X254" t="s">
         <v>44</v>
       </c>
@@ -63598,6 +64112,9 @@
       <c r="V255" s="1">
         <v>41505</v>
       </c>
+      <c r="W255" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X255" t="s">
         <v>44</v>
       </c>
@@ -63705,6 +64222,9 @@
       <c r="V256" s="1">
         <v>42009</v>
       </c>
+      <c r="W256" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X256" t="s">
         <v>44</v>
       </c>
@@ -63812,6 +64332,9 @@
       <c r="V257" s="1">
         <v>42125</v>
       </c>
+      <c r="W257" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X257" t="s">
         <v>44</v>
       </c>
@@ -64029,6 +64552,9 @@
       <c r="V259" s="1">
         <v>41911</v>
       </c>
+      <c r="W259" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X259" t="s">
         <v>44</v>
       </c>
@@ -64136,6 +64662,9 @@
       <c r="V260" s="1">
         <v>41777</v>
       </c>
+      <c r="W260" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X260" t="s">
         <v>44</v>
       </c>
@@ -64353,6 +64882,9 @@
       <c r="V262" s="1">
         <v>41589</v>
       </c>
+      <c r="W262" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X262" t="s">
         <v>44</v>
       </c>
@@ -64460,6 +64992,9 @@
       <c r="V263" s="1">
         <v>40704</v>
       </c>
+      <c r="W263" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X263" t="s">
         <v>44</v>
       </c>
@@ -64567,6 +65102,9 @@
       <c r="V264" s="1">
         <v>42551</v>
       </c>
+      <c r="W264" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X264" t="s">
         <v>44</v>
       </c>
@@ -64674,6 +65212,9 @@
       <c r="V265" s="1">
         <v>40959</v>
       </c>
+      <c r="W265" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X265" t="s">
         <v>44</v>
       </c>
@@ -64781,6 +65322,9 @@
       <c r="V266" s="1">
         <v>41184</v>
       </c>
+      <c r="W266" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X266" t="s">
         <v>44</v>
       </c>
@@ -64998,6 +65542,9 @@
       <c r="V268" s="1">
         <v>40553</v>
       </c>
+      <c r="W268" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X268" t="s">
         <v>44</v>
       </c>
@@ -65105,6 +65652,9 @@
       <c r="V269" s="1">
         <v>41771</v>
       </c>
+      <c r="W269" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X269" t="s">
         <v>44</v>
       </c>
@@ -65212,6 +65762,9 @@
       <c r="V270" s="1">
         <v>41911</v>
       </c>
+      <c r="W270" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X270" t="s">
         <v>44</v>
       </c>
@@ -65319,6 +65872,9 @@
       <c r="V271" s="1">
         <v>41687</v>
       </c>
+      <c r="W271" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X271" t="s">
         <v>44</v>
       </c>
@@ -65426,6 +65982,9 @@
       <c r="V272" s="1">
         <v>40448</v>
       </c>
+      <c r="W272" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X272" t="s">
         <v>44</v>
       </c>
@@ -65533,6 +66092,9 @@
       <c r="V273" s="1">
         <v>39821</v>
       </c>
+      <c r="W273" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X273" t="s">
         <v>44</v>
       </c>
@@ -65640,6 +66202,9 @@
       <c r="V274" s="1">
         <v>42009</v>
       </c>
+      <c r="W274" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X274" t="s">
         <v>44</v>
       </c>
@@ -65747,6 +66312,9 @@
       <c r="V275" s="1">
         <v>41043</v>
       </c>
+      <c r="W275" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X275" t="s">
         <v>44</v>
       </c>
@@ -65854,6 +66422,9 @@
       <c r="V276" s="1">
         <v>41827</v>
       </c>
+      <c r="W276" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X276" t="s">
         <v>44</v>
       </c>
@@ -65961,6 +66532,9 @@
       <c r="V277" s="1">
         <v>42845</v>
       </c>
+      <c r="W277" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X277" t="s">
         <v>44</v>
       </c>
@@ -66288,6 +66862,9 @@
       <c r="V280" s="1">
         <v>41911</v>
       </c>
+      <c r="W280" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X280" t="s">
         <v>44</v>
       </c>
@@ -66615,6 +67192,9 @@
       <c r="V283" s="1">
         <v>41323</v>
       </c>
+      <c r="W283" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X283" t="s">
         <v>44</v>
       </c>
@@ -66722,6 +67302,9 @@
       <c r="V284" s="1">
         <v>38726</v>
       </c>
+      <c r="W284" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X284" t="s">
         <v>44</v>
       </c>
@@ -66829,6 +67412,9 @@
       <c r="V285" s="1">
         <v>41687</v>
       </c>
+      <c r="W285" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X285" t="s">
         <v>44</v>
       </c>
@@ -67266,6 +67852,9 @@
       <c r="V289" s="1">
         <v>42093</v>
       </c>
+      <c r="W289" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X289" t="s">
         <v>44</v>
       </c>
@@ -67373,6 +67962,9 @@
       <c r="V290" s="1">
         <v>40729</v>
       </c>
+      <c r="W290" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X290" t="s">
         <v>44</v>
       </c>
@@ -67590,6 +68182,9 @@
       <c r="V292" s="1">
         <v>40756</v>
       </c>
+      <c r="W292" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X292" t="s">
         <v>44</v>
       </c>
@@ -67697,6 +68292,9 @@
       <c r="V293" s="1">
         <v>40973</v>
       </c>
+      <c r="W293" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X293" t="s">
         <v>44</v>
       </c>
@@ -68024,6 +68622,9 @@
       <c r="V296" s="1">
         <v>42190</v>
       </c>
+      <c r="W296" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X296" t="s">
         <v>44</v>
       </c>
@@ -68131,6 +68732,9 @@
       <c r="V297" s="1">
         <v>41869</v>
       </c>
+      <c r="W297" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X297" t="s">
         <v>44</v>
       </c>
@@ -68458,6 +69062,9 @@
       <c r="V300" s="1">
         <v>42781</v>
       </c>
+      <c r="W300" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X300" t="s">
         <v>44</v>
       </c>
@@ -68565,6 +69172,9 @@
       <c r="V301" s="1">
         <v>42093</v>
       </c>
+      <c r="W301" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X301" t="s">
         <v>44</v>
       </c>
@@ -69222,6 +69832,9 @@
       <c r="V307" s="1">
         <v>41911</v>
       </c>
+      <c r="W307" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X307" t="s">
         <v>44</v>
       </c>
@@ -69329,6 +69942,9 @@
       <c r="V308" s="1">
         <v>41827</v>
       </c>
+      <c r="W308" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X308" t="s">
         <v>44</v>
       </c>
@@ -69546,6 +70162,9 @@
       <c r="V310" s="1">
         <v>40278</v>
       </c>
+      <c r="W310" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X310" t="s">
         <v>44</v>
       </c>
@@ -69653,6 +70272,9 @@
       <c r="V311" s="1">
         <v>42093</v>
       </c>
+      <c r="W311" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X311" t="s">
         <v>44</v>
       </c>
@@ -69760,6 +70382,9 @@
       <c r="V312" s="1">
         <v>41911</v>
       </c>
+      <c r="W312" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="X312" t="s">
         <v>44</v>
       </c>
@@ -69801,7 +70426,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AJ312" xr:uid="{3C1C7566-FF8C-4B87-AFAC-D0B14E4AA402}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>